<commit_message>
Done bits of Part C
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,18 +17,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="39">
   <si>
     <t>50Hz</t>
   </si>
   <si>
     <t>45Hz</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Student number</t>
   </si>
   <si>
     <t>Motor Model</t>
@@ -44,6 +38,9 @@
   </si>
   <si>
     <t>W</t>
+  </si>
+  <si>
+    <t>Theoretical</t>
   </si>
   <si>
     <t>Braking %</t>
@@ -73,10 +70,19 @@
     <t>Power</t>
   </si>
   <si>
+    <t>Torque</t>
+  </si>
+  <si>
+    <t>3?</t>
+  </si>
+  <si>
     <t>40Hz</t>
   </si>
   <si>
     <t>35Hz</t>
+  </si>
+  <si>
+    <t>2?</t>
   </si>
   <si>
     <t>30Hz</t>
@@ -101,9 +107,6 @@
   </si>
   <si>
     <t>Torque %)</t>
-  </si>
-  <si>
-    <t>Torque</t>
   </si>
   <si>
     <t>45 Stalled</t>
@@ -140,7 +143,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -182,6 +185,12 @@
       <family val="2"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -195,7 +204,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -206,6 +215,13 @@
     <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -246,7 +262,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -255,11 +271,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -268,14 +288,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -369,7 +381,7 @@
               <a:rPr sz="1300">
                 <a:latin typeface="Arial"/>
               </a:rPr>
-              <a:t>DSP Torque Speed Curves</a:t>
+              <a:t>DSP Speed Torque Curves</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1827,11 +1839,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="58858016"/>
-        <c:axId val="64258464"/>
+        <c:axId val="16562524"/>
+        <c:axId val="93310197"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="58858016"/>
+        <c:axId val="16562524"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1847,7 +1859,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900">
+                  <a:rPr b="1" sz="900">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Speed (RPM)</a:t>
@@ -1867,11 +1879,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="64258464"/>
+        <c:crossAx val="93310197"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64258464"/>
+        <c:axId val="93310197"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1896,7 +1908,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900">
+                  <a:rPr b="1" sz="900">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Torque (Nm)</a:t>
@@ -1916,7 +1928,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="58858016"/>
+        <c:crossAx val="16562524"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -1968,7 +1980,7 @@
               <a:rPr sz="1300">
                 <a:latin typeface="Arial"/>
               </a:rPr>
-              <a:t>Drivewindows Torque Speed Curves</a:t>
+              <a:t>Model Speed Torque Curves</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3426,11 +3438,614 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="16483134"/>
-        <c:axId val="89390131"/>
+        <c:axId val="58930307"/>
+        <c:axId val="89963729"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="16483134"/>
+        <c:axId val="58930307"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="900">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Speed (RPM)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="89963729"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="89963729"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="900">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Torque (%)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="58930307"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr sz="1300">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>50 Hz Model, Actual, and Theoretical Torque Speed Curves</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$J$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Theoretical</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ee4000"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$J$4:$J$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1385</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$K$4:$K$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>3.79</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ffd320"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ee4000"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$G$4:$G$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>1496</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1496</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1495</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1495</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1494</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1494</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1494</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1493</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1492</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1491</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1490</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1488</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1484</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1480</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1473</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1459</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1447</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1424</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1392</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1342</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1290</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1109</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$F$4:$F$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>-0.012</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.012</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.052</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.046</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.074</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.159</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.21</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.263</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.355</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.542</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.085</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.68</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.193</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.95</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.21</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6.116</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>7.26</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Motor Model</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ee4000"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$C$4:$C$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>1489.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1489.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1489.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1489.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1489.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1488.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1488.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1488.1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1487.1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1486.4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1485.9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1484.4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1481.9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1479</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1474.1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1464.9</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1457</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1443.9</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1427.2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1401.9</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1380.3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1341</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>820.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$4:$B$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>18.93</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19.32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19.69</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20.09</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>21.04</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22.18</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>22.58</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>23.98</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25.73</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>26.42</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>29.28</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>34.42</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>39.57</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>48.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>65.94</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>80.78</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>105.31</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>136.51</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>184.28</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>224.86</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>298.76</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>444.74</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="11676663"/>
+        <c:axId val="27775071"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="11676663"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3466,25 +4081,18 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="89390131"/>
+        <c:crossAx val="27775071"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="89390131"/>
+        <c:axId val="27775071"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="500"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -3515,8 +4123,10 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="16483134"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="11676663"/>
+        <c:crosses val="max"/>
+        <c:majorUnit val="50"/>
+        <c:minorUnit val="25"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -3550,20 +4160,415 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr sz="1300">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>50 Hz Actual and Theoretical Torque Speed Curves</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$J$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Theoretical</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ee4000"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="004586"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="0"/>
+            <c:backward val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$J$4:$J$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1385</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$K$4:$K$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>3.79</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ffd320"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ee4000"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="ffd320"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="0"/>
+            <c:backward val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$G$4:$G$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>1496</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1496</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1495</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1495</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1494</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1494</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1494</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1493</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1492</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1491</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1490</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1488</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1484</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1480</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1473</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1459</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1447</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$F$4:$F$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>-0.012</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.012</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.052</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.046</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.074</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.159</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.21</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.263</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.355</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.542</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.085</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.68</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.193</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="77016186"/>
+        <c:axId val="96454864"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="77016186"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr sz="900">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Speed (RPM)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="96454864"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="96454864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr sz="900">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Torque(Nm)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="77016186"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>610200</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>21600</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>-360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>861120</xdr:colOff>
+      <xdr:colOff>888120</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>78120</xdr:rowOff>
+      <xdr:rowOff>84240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3571,8 +4576,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="15432120" y="709200"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="15658200" y="700560"/>
+        <a:ext cx="5759280" cy="3239280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3585,15 +4590,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>33840</xdr:colOff>
+      <xdr:colOff>61200</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>119880</xdr:rowOff>
+      <xdr:rowOff>126360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>900720</xdr:colOff>
+      <xdr:colOff>927720</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>29520</xdr:rowOff>
+      <xdr:rowOff>35640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3601,12 +4606,72 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="15471720" y="4165920"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="15697800" y="4157280"/>
+        <a:ext cx="5759280" cy="3269520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>252000</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>21240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>1029960</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>117360</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="15888600" y="7763040"/>
+        <a:ext cx="5670720" cy="3265920"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>216720</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>21600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>126360</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>132840</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="23418720" y="722520"/>
+        <a:ext cx="8533080" cy="3265920"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3620,10 +4685,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AC111"/>
+  <dimension ref="A1:AT111"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F27" activeCellId="0" sqref="F27"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="R1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AB1" activeCellId="0" sqref="AB1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3634,7 +4699,9 @@
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.1377551020408"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.4183673469388"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.0051020408163"/>
-    <col collapsed="false" hidden="false" max="17" min="7" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.5459183673469"/>
+    <col collapsed="false" hidden="false" max="17" min="11" style="0" width="8.72959183673469"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="0" width="13.5714285714286"/>
     <col collapsed="false" hidden="false" max="26" min="19" style="0" width="8.72959183673469"/>
     <col collapsed="false" hidden="false" max="27" min="27" style="0" width="34.4234693877551"/>
@@ -3642,109 +4709,112 @@
     <col collapsed="false" hidden="false" max="1025" min="29" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="N1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="AA1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB1" s="0" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="I2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="J2" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="0" t="s">
-        <v>8</v>
-      </c>
       <c r="N2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="S2" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="T2" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="0" t="s">
+      <c r="U2" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="T2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="U2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="AA2" s="2"/>
+      <c r="AA2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="C3" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="F3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="H3" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="I3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="J3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="0" t="s">
         <v>17</v>
       </c>
       <c r="M3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="N3" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="0" t="s">
+      <c r="O3" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="O3" s="0" t="s">
+      <c r="P3" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="P3" s="0" t="s">
+      <c r="Q3" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="Q3" s="0" t="s">
+      <c r="R3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="S3" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="S3" s="0" t="s">
+      <c r="T3" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="T3" s="0" t="s">
+      <c r="U3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="U3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA3" s="2"/>
+      <c r="AA3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -3772,8 +4842,14 @@
         <f aca="false">D4</f>
         <v>1.02</v>
       </c>
-      <c r="I4" s="0" t="n">
+      <c r="I4" s="2" t="n">
         <v>2</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>1385</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>3.79</v>
       </c>
       <c r="M4" s="0" t="n">
         <v>0</v>
@@ -3803,7 +4879,7 @@
       <c r="U4" s="0" t="n">
         <v>0.29</v>
       </c>
-      <c r="AA4" s="2"/>
+      <c r="AA4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -3831,8 +4907,14 @@
         <f aca="false">D5</f>
         <v>1.02</v>
       </c>
-      <c r="I5" s="0" t="n">
+      <c r="I5" s="2" t="n">
         <v>1.14</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>1500</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="M5" s="0" t="n">
         <v>2</v>
@@ -3862,7 +4944,7 @@
       <c r="U5" s="0" t="n">
         <v>0.32</v>
       </c>
-      <c r="AA5" s="2"/>
+      <c r="AA5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -3890,7 +4972,7 @@
         <f aca="false">D6</f>
         <v>1.02</v>
       </c>
-      <c r="I6" s="0" t="n">
+      <c r="I6" s="2" t="n">
         <v>0.13</v>
       </c>
       <c r="M6" s="0" t="n">
@@ -3921,7 +5003,7 @@
       <c r="U6" s="0" t="n">
         <v>0.84</v>
       </c>
-      <c r="AA6" s="2"/>
+      <c r="AA6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -3949,7 +5031,7 @@
         <f aca="false">D7</f>
         <v>1.02</v>
       </c>
-      <c r="I7" s="0" t="n">
+      <c r="I7" s="2" t="n">
         <v>1.7</v>
       </c>
       <c r="M7" s="0" t="n">
@@ -3980,7 +5062,7 @@
       <c r="U7" s="0" t="n">
         <v>2.72</v>
       </c>
-      <c r="AA7" s="2"/>
+      <c r="AA7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -4008,7 +5090,7 @@
         <f aca="false">D8</f>
         <v>1.02</v>
       </c>
-      <c r="I8" s="0" t="n">
+      <c r="I8" s="2" t="n">
         <v>8.3</v>
       </c>
       <c r="M8" s="0" t="n">
@@ -4039,7 +5121,7 @@
       <c r="U8" s="0" t="n">
         <v>5.15</v>
       </c>
-      <c r="AA8" s="2"/>
+      <c r="AA8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
@@ -4054,10 +5136,10 @@
       <c r="D9" s="0" t="n">
         <v>1.02</v>
       </c>
-      <c r="E9" s="3" t="n">
+      <c r="E9" s="4" t="n">
         <v>20.64</v>
       </c>
-      <c r="F9" s="4" t="n">
+      <c r="F9" s="5" t="n">
         <v>0.046</v>
       </c>
       <c r="G9" s="0" t="n">
@@ -4067,7 +5149,7 @@
         <f aca="false">D9</f>
         <v>1.02</v>
       </c>
-      <c r="I9" s="0" t="n">
+      <c r="I9" s="2" t="n">
         <v>7.3</v>
       </c>
       <c r="M9" s="0" t="n">
@@ -4082,10 +5164,10 @@
       <c r="P9" s="0" t="n">
         <v>0.99</v>
       </c>
-      <c r="Q9" s="3" t="n">
+      <c r="Q9" s="4" t="n">
         <v>19.88</v>
       </c>
-      <c r="R9" s="4" t="n">
+      <c r="R9" s="5" t="n">
         <v>0.058</v>
       </c>
       <c r="S9" s="0" t="n">
@@ -4098,7 +5180,7 @@
       <c r="U9" s="0" t="n">
         <v>8.16</v>
       </c>
-      <c r="AA9" s="2"/>
+      <c r="AA9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
@@ -4113,10 +5195,10 @@
       <c r="D10" s="0" t="n">
         <v>1.02</v>
       </c>
-      <c r="E10" s="3" t="n">
+      <c r="E10" s="4" t="n">
         <v>21.42</v>
       </c>
-      <c r="F10" s="4" t="n">
+      <c r="F10" s="5" t="n">
         <v>0.074</v>
       </c>
       <c r="G10" s="0" t="n">
@@ -4126,7 +5208,7 @@
         <f aca="false">D10</f>
         <v>1.02</v>
       </c>
-      <c r="I10" s="0" t="n">
+      <c r="I10" s="2" t="n">
         <v>11.5</v>
       </c>
       <c r="M10" s="0" t="n">
@@ -4141,10 +5223,10 @@
       <c r="P10" s="0" t="n">
         <v>0.99</v>
       </c>
-      <c r="Q10" s="3" t="n">
+      <c r="Q10" s="4" t="n">
         <v>20.72</v>
       </c>
-      <c r="R10" s="4" t="n">
+      <c r="R10" s="5" t="n">
         <v>0.085</v>
       </c>
       <c r="S10" s="0" t="n">
@@ -4157,7 +5239,7 @@
       <c r="U10" s="0" t="n">
         <v>11.92</v>
       </c>
-      <c r="AA10" s="2"/>
+      <c r="AA10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
@@ -4172,10 +5254,10 @@
       <c r="D11" s="0" t="n">
         <v>1.02</v>
       </c>
-      <c r="E11" s="3" t="n">
+      <c r="E11" s="4" t="n">
         <v>23.36</v>
       </c>
-      <c r="F11" s="4" t="n">
+      <c r="F11" s="5" t="n">
         <v>0.11</v>
       </c>
       <c r="G11" s="0" t="n">
@@ -4185,7 +5267,7 @@
         <f aca="false">D11</f>
         <v>1.02</v>
       </c>
-      <c r="I11" s="0" t="n">
+      <c r="I11" s="2" t="n">
         <v>17</v>
       </c>
       <c r="M11" s="0" t="n">
@@ -4200,10 +5282,10 @@
       <c r="P11" s="0" t="n">
         <v>0.99</v>
       </c>
-      <c r="Q11" s="3" t="n">
+      <c r="Q11" s="4" t="n">
         <v>21.41</v>
       </c>
-      <c r="R11" s="4" t="n">
+      <c r="R11" s="5" t="n">
         <v>0.121</v>
       </c>
       <c r="S11" s="0" t="n">
@@ -4216,7 +5298,7 @@
       <c r="U11" s="0" t="n">
         <v>10.8</v>
       </c>
-      <c r="AA11" s="2"/>
+      <c r="AA11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
@@ -4231,10 +5313,10 @@
       <c r="D12" s="0" t="n">
         <v>1.01</v>
       </c>
-      <c r="E12" s="3" t="n">
+      <c r="E12" s="4" t="n">
         <v>24.68</v>
       </c>
-      <c r="F12" s="4" t="n">
+      <c r="F12" s="5" t="n">
         <v>0.159</v>
       </c>
       <c r="G12" s="0" t="n">
@@ -4244,7 +5326,7 @@
         <f aca="false">D12</f>
         <v>1.01</v>
       </c>
-      <c r="I12" s="0" t="n">
+      <c r="I12" s="2" t="n">
         <v>24.7</v>
       </c>
       <c r="M12" s="0" t="n">
@@ -4259,10 +5341,10 @@
       <c r="P12" s="0" t="n">
         <v>0.99</v>
       </c>
-      <c r="Q12" s="3" t="n">
+      <c r="Q12" s="4" t="n">
         <v>22.41</v>
       </c>
-      <c r="R12" s="4" t="n">
+      <c r="R12" s="5" t="n">
         <v>0.164</v>
       </c>
       <c r="S12" s="0" t="n">
@@ -4275,7 +5357,7 @@
       <c r="U12" s="0" t="n">
         <v>22.98</v>
       </c>
-      <c r="AA12" s="2"/>
+      <c r="AA12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
@@ -4290,10 +5372,10 @@
       <c r="D13" s="0" t="n">
         <v>1.01</v>
       </c>
-      <c r="E13" s="3" t="n">
+      <c r="E13" s="4" t="n">
         <v>26.67</v>
       </c>
-      <c r="F13" s="4" t="n">
+      <c r="F13" s="5" t="n">
         <v>0.21</v>
       </c>
       <c r="G13" s="0" t="n">
@@ -4303,7 +5385,7 @@
         <f aca="false">D13</f>
         <v>1.01</v>
       </c>
-      <c r="I13" s="0" t="n">
+      <c r="I13" s="2" t="n">
         <v>32.9</v>
       </c>
       <c r="M13" s="0" t="n">
@@ -4318,10 +5400,10 @@
       <c r="P13" s="0" t="n">
         <v>0.99</v>
       </c>
-      <c r="Q13" s="3" t="n">
+      <c r="Q13" s="4" t="n">
         <v>23.91</v>
       </c>
-      <c r="R13" s="4" t="n">
+      <c r="R13" s="5" t="n">
         <v>0.214</v>
       </c>
       <c r="S13" s="0" t="n">
@@ -4334,7 +5416,7 @@
       <c r="U13" s="0" t="n">
         <v>30.03</v>
       </c>
-      <c r="AA13" s="2"/>
+      <c r="AA13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
@@ -4349,10 +5431,10 @@
       <c r="D14" s="0" t="n">
         <v>1.02</v>
       </c>
-      <c r="E14" s="3" t="n">
+      <c r="E14" s="4" t="n">
         <v>27.39</v>
       </c>
-      <c r="F14" s="4" t="n">
+      <c r="F14" s="5" t="n">
         <v>0.263</v>
       </c>
       <c r="G14" s="0" t="n">
@@ -4362,7 +5444,7 @@
         <f aca="false">D14</f>
         <v>1.02</v>
       </c>
-      <c r="I14" s="0" t="n">
+      <c r="I14" s="2" t="n">
         <v>41</v>
       </c>
       <c r="M14" s="0" t="n">
@@ -4377,10 +5459,10 @@
       <c r="P14" s="0" t="n">
         <v>0.99</v>
       </c>
-      <c r="Q14" s="3" t="n">
+      <c r="Q14" s="4" t="n">
         <v>25.7</v>
       </c>
-      <c r="R14" s="4" t="n">
+      <c r="R14" s="5" t="n">
         <v>0.228</v>
       </c>
       <c r="S14" s="0" t="n">
@@ -4393,7 +5475,13 @@
       <c r="U14" s="0" t="n">
         <v>39.07</v>
       </c>
-      <c r="AA14" s="2"/>
+      <c r="AA14" s="3"/>
+      <c r="AC14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT14" s="0" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
@@ -4408,10 +5496,10 @@
       <c r="D15" s="0" t="n">
         <v>1.02</v>
       </c>
-      <c r="E15" s="3" t="n">
+      <c r="E15" s="4" t="n">
         <v>30.29</v>
       </c>
-      <c r="F15" s="4" t="n">
+      <c r="F15" s="5" t="n">
         <v>0.355</v>
       </c>
       <c r="G15" s="0" t="n">
@@ -4421,7 +5509,7 @@
         <f aca="false">D15</f>
         <v>1.02</v>
       </c>
-      <c r="I15" s="0" t="n">
+      <c r="I15" s="2" t="n">
         <v>55.2</v>
       </c>
       <c r="M15" s="0" t="n">
@@ -4436,10 +5524,10 @@
       <c r="P15" s="0" t="n">
         <v>0.98</v>
       </c>
-      <c r="Q15" s="3" t="n">
+      <c r="Q15" s="4" t="n">
         <v>27.6</v>
       </c>
-      <c r="R15" s="4" t="n">
+      <c r="R15" s="5" t="n">
         <v>0.37</v>
       </c>
       <c r="S15" s="0" t="n">
@@ -4452,7 +5540,10 @@
       <c r="U15" s="0" t="n">
         <v>15.72</v>
       </c>
-      <c r="AA15" s="2"/>
+      <c r="AA15" s="3"/>
+      <c r="AC15" s="0" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
@@ -4467,10 +5558,10 @@
       <c r="D16" s="0" t="n">
         <v>1.02</v>
       </c>
-      <c r="E16" s="3" t="n">
+      <c r="E16" s="4" t="n">
         <v>35.78</v>
       </c>
-      <c r="F16" s="4" t="n">
+      <c r="F16" s="5" t="n">
         <v>0.542</v>
       </c>
       <c r="G16" s="0" t="n">
@@ -4480,7 +5571,7 @@
         <f aca="false">D16</f>
         <v>1.02</v>
       </c>
-      <c r="I16" s="0" t="n">
+      <c r="I16" s="2" t="n">
         <v>84.3</v>
       </c>
       <c r="M16" s="0" t="n">
@@ -4495,10 +5586,10 @@
       <c r="P16" s="0" t="n">
         <v>0.99</v>
       </c>
-      <c r="Q16" s="3" t="n">
+      <c r="Q16" s="4" t="n">
         <v>31.48</v>
       </c>
-      <c r="R16" s="4" t="n">
+      <c r="R16" s="5" t="n">
         <v>0.526</v>
       </c>
       <c r="S16" s="0" t="n">
@@ -4511,7 +5602,7 @@
       <c r="U16" s="0" t="n">
         <v>73.33</v>
       </c>
-      <c r="AA16" s="2"/>
+      <c r="AA16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
@@ -4526,10 +5617,10 @@
       <c r="D17" s="0" t="n">
         <v>1.03</v>
       </c>
-      <c r="E17" s="3" t="n">
+      <c r="E17" s="4" t="n">
         <v>41.34</v>
       </c>
-      <c r="F17" s="4" t="n">
+      <c r="F17" s="5" t="n">
         <v>0.74</v>
       </c>
       <c r="G17" s="0" t="n">
@@ -4539,7 +5630,7 @@
         <f aca="false">D17</f>
         <v>1.03</v>
       </c>
-      <c r="I17" s="0" t="n">
+      <c r="I17" s="2" t="n">
         <v>114.8</v>
       </c>
       <c r="M17" s="0" t="n">
@@ -4554,10 +5645,10 @@
       <c r="P17" s="0" t="n">
         <v>0.99</v>
       </c>
-      <c r="Q17" s="3" t="n">
+      <c r="Q17" s="4" t="n">
         <v>37.9</v>
       </c>
-      <c r="R17" s="4" t="n">
+      <c r="R17" s="5" t="n">
         <v>0.765</v>
       </c>
       <c r="S17" s="0" t="n">
@@ -4570,7 +5661,7 @@
       <c r="U17" s="0" t="n">
         <v>106.4</v>
       </c>
-      <c r="AA17" s="2"/>
+      <c r="AA17" s="3"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
@@ -4585,10 +5676,10 @@
       <c r="D18" s="0" t="n">
         <v>1.04</v>
       </c>
-      <c r="E18" s="3" t="n">
+      <c r="E18" s="4" t="n">
         <v>50.75</v>
       </c>
-      <c r="F18" s="4" t="n">
+      <c r="F18" s="5" t="n">
         <v>1.085</v>
       </c>
       <c r="G18" s="0" t="n">
@@ -4598,7 +5689,7 @@
         <f aca="false">D18</f>
         <v>1.04</v>
       </c>
-      <c r="I18" s="0" t="n">
+      <c r="I18" s="2" t="n">
         <v>167.5</v>
       </c>
       <c r="M18" s="0" t="n">
@@ -4613,10 +5704,10 @@
       <c r="P18" s="0" t="n">
         <v>1.01</v>
       </c>
-      <c r="Q18" s="3" t="n">
+      <c r="Q18" s="4" t="n">
         <v>46.54</v>
       </c>
-      <c r="R18" s="4" t="n">
+      <c r="R18" s="5" t="n">
         <v>1.118</v>
       </c>
       <c r="S18" s="0" t="n">
@@ -4634,19 +5725,19 @@
       <c r="A19" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="B19" s="5" t="n">
+      <c r="B19" s="6" t="n">
         <v>65.94</v>
       </c>
-      <c r="C19" s="5" t="n">
+      <c r="C19" s="6" t="n">
         <v>1464.9</v>
       </c>
       <c r="D19" s="6" t="n">
         <v>1.09</v>
       </c>
-      <c r="E19" s="3" t="n">
+      <c r="E19" s="4" t="n">
         <v>68.9</v>
       </c>
-      <c r="F19" s="4" t="n">
+      <c r="F19" s="5" t="n">
         <v>1.68</v>
       </c>
       <c r="G19" s="0" t="n">
@@ -4656,25 +5747,25 @@
         <f aca="false">D19</f>
         <v>1.09</v>
       </c>
-      <c r="I19" s="0" t="n">
+      <c r="I19" s="2" t="n">
         <v>258</v>
       </c>
       <c r="M19" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="N19" s="5" t="n">
+      <c r="N19" s="6" t="n">
         <v>64.25</v>
       </c>
-      <c r="O19" s="5" t="n">
+      <c r="O19" s="6" t="n">
         <v>1315.8</v>
       </c>
       <c r="P19" s="6" t="n">
         <v>1.05</v>
       </c>
-      <c r="Q19" s="3" t="n">
+      <c r="Q19" s="4" t="n">
         <v>60.26</v>
       </c>
-      <c r="R19" s="4" t="n">
+      <c r="R19" s="5" t="n">
         <v>1.61</v>
       </c>
       <c r="S19" s="0" t="n">
@@ -4687,7 +5778,7 @@
       <c r="U19" s="0" t="n">
         <v>221.1</v>
       </c>
-      <c r="AA19" s="2"/>
+      <c r="AA19" s="3"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
@@ -4702,10 +5793,10 @@
       <c r="D20" s="6" t="n">
         <v>1.15</v>
       </c>
-      <c r="E20" s="3" t="n">
+      <c r="E20" s="4" t="n">
         <v>84.14</v>
       </c>
-      <c r="F20" s="4" t="n">
+      <c r="F20" s="5" t="n">
         <v>2.193</v>
       </c>
       <c r="G20" s="0" t="n">
@@ -4715,7 +5806,7 @@
         <f aca="false">D20</f>
         <v>1.15</v>
       </c>
-      <c r="I20" s="0" t="n">
+      <c r="I20" s="2" t="n">
         <v>332.2</v>
       </c>
       <c r="M20" s="0" t="n">
@@ -4730,10 +5821,10 @@
       <c r="P20" s="6" t="n">
         <v>1.13</v>
       </c>
-      <c r="Q20" s="3" t="n">
+      <c r="Q20" s="4" t="n">
         <v>77.92</v>
       </c>
-      <c r="R20" s="4" t="n">
+      <c r="R20" s="5" t="n">
         <v>2.26</v>
       </c>
       <c r="S20" s="0" t="n">
@@ -4746,7 +5837,7 @@
       <c r="U20" s="0" t="n">
         <v>306.4</v>
       </c>
-      <c r="AA20" s="2"/>
+      <c r="AA20" s="3"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
@@ -4761,10 +5852,10 @@
       <c r="D21" s="6" t="n">
         <v>1.31</v>
       </c>
-      <c r="E21" s="3" t="n">
+      <c r="E21" s="4" t="n">
         <v>108.95</v>
       </c>
-      <c r="F21" s="4" t="n">
+      <c r="F21" s="5" t="n">
         <v>3</v>
       </c>
       <c r="G21" s="0" t="n">
@@ -4774,7 +5865,7 @@
         <f aca="false">D21</f>
         <v>1.31</v>
       </c>
-      <c r="I21" s="0" t="n">
+      <c r="I21" s="2" t="n">
         <v>449</v>
       </c>
       <c r="M21" s="0" t="n">
@@ -4789,10 +5880,10 @@
       <c r="P21" s="6" t="n">
         <v>1.28</v>
       </c>
-      <c r="Q21" s="3" t="n">
+      <c r="Q21" s="4" t="n">
         <v>100.6</v>
       </c>
-      <c r="R21" s="4" t="n">
+      <c r="R21" s="5" t="n">
         <v>3.052</v>
       </c>
       <c r="S21" s="0" t="n">
@@ -4805,7 +5896,7 @@
       <c r="U21" s="0" t="n">
         <v>405.3</v>
       </c>
-      <c r="AA21" s="2"/>
+      <c r="AA21" s="3"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
@@ -4820,10 +5911,10 @@
       <c r="D22" s="6" t="n">
         <v>1.5</v>
       </c>
-      <c r="E22" s="3" t="n">
+      <c r="E22" s="4" t="n">
         <v>139.96</v>
       </c>
-      <c r="F22" s="4" t="n">
+      <c r="F22" s="5" t="n">
         <v>3.95</v>
       </c>
       <c r="G22" s="0" t="n">
@@ -4833,7 +5924,7 @@
         <f aca="false">D22</f>
         <v>1.5</v>
       </c>
-      <c r="I22" s="0" t="n">
+      <c r="I22" s="2" t="n">
         <v>578</v>
       </c>
       <c r="M22" s="0" t="n">
@@ -4848,10 +5939,10 @@
       <c r="P22" s="6" t="n">
         <v>1.5</v>
       </c>
-      <c r="Q22" s="3" t="n">
+      <c r="Q22" s="4" t="n">
         <v>129.53</v>
       </c>
-      <c r="R22" s="4" t="n">
+      <c r="R22" s="5" t="n">
         <v>3.98</v>
       </c>
       <c r="S22" s="0" t="n">
@@ -4864,8 +5955,8 @@
       <c r="U22" s="0" t="n">
         <v>515.9</v>
       </c>
-      <c r="AA22" s="2"/>
-      <c r="AC22" s="2"/>
+      <c r="AA22" s="3"/>
+      <c r="AC22" s="3"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
@@ -4880,10 +5971,10 @@
       <c r="D23" s="6" t="n">
         <v>1.87</v>
       </c>
-      <c r="E23" s="3" t="n">
+      <c r="E23" s="4" t="n">
         <v>185.76</v>
       </c>
-      <c r="F23" s="4" t="n">
+      <c r="F23" s="5" t="n">
         <v>5.21</v>
       </c>
       <c r="G23" s="0" t="n">
@@ -4893,7 +5984,7 @@
         <f aca="false">D23</f>
         <v>1.87</v>
       </c>
-      <c r="I23" s="0" t="n">
+      <c r="I23" s="2" t="n">
         <v>734</v>
       </c>
       <c r="M23" s="0" t="n">
@@ -4908,10 +5999,10 @@
       <c r="P23" s="6" t="n">
         <v>1.93</v>
       </c>
-      <c r="Q23" s="3" t="n">
+      <c r="Q23" s="4" t="n">
         <v>176.88</v>
       </c>
-      <c r="R23" s="4" t="n">
+      <c r="R23" s="5" t="n">
         <v>5.01</v>
       </c>
       <c r="S23" s="0" t="n">
@@ -4938,10 +6029,10 @@
       <c r="D24" s="6" t="n">
         <v>2.26</v>
       </c>
-      <c r="E24" s="3" t="n">
+      <c r="E24" s="4" t="n">
         <v>223.76</v>
       </c>
-      <c r="F24" s="4" t="n">
+      <c r="F24" s="5" t="n">
         <v>6.116</v>
       </c>
       <c r="G24" s="0" t="n">
@@ -4951,7 +6042,7 @@
         <f aca="false">D24</f>
         <v>2.26</v>
       </c>
-      <c r="I24" s="0" t="n">
+      <c r="I24" s="2" t="n">
         <v>825</v>
       </c>
       <c r="M24" s="0" t="n">
@@ -4966,10 +6057,10 @@
       <c r="P24" s="6" t="n">
         <v>2.23</v>
       </c>
-      <c r="Q24" s="3" t="n">
+      <c r="Q24" s="4" t="n">
         <v>204.82</v>
       </c>
-      <c r="R24" s="4" t="n">
+      <c r="R24" s="5" t="n">
         <v>6.106</v>
       </c>
       <c r="S24" s="0" t="n">
@@ -4996,10 +6087,10 @@
       <c r="D25" s="6" t="n">
         <v>2.85</v>
       </c>
-      <c r="E25" s="3" t="n">
+      <c r="E25" s="4" t="n">
         <v>288.85</v>
       </c>
-      <c r="F25" s="4" t="n">
+      <c r="F25" s="5" t="n">
         <v>7.26</v>
       </c>
       <c r="G25" s="0" t="n">
@@ -5009,7 +6100,7 @@
         <f aca="false">D25</f>
         <v>2.85</v>
       </c>
-      <c r="I25" s="0" t="n">
+      <c r="I25" s="2" t="n">
         <v>810</v>
       </c>
       <c r="M25" s="0" t="n">
@@ -5024,7 +6115,7 @@
       <c r="P25" s="6" t="n">
         <v>2.9</v>
       </c>
-      <c r="Q25" s="7" t="n">
+      <c r="Q25" s="4" t="n">
         <v>262.93</v>
       </c>
       <c r="R25" s="1" t="n">
@@ -5054,10 +6145,10 @@
       <c r="D26" s="6" t="n">
         <v>4.18</v>
       </c>
-      <c r="E26" s="3" t="n">
+      <c r="E26" s="4" t="n">
         <v>264.66</v>
       </c>
-      <c r="F26" s="4" t="n">
+      <c r="F26" s="5" t="n">
         <v>5.4</v>
       </c>
       <c r="G26" s="0" t="n">
@@ -5066,7 +6157,7 @@
       <c r="H26" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="I26" s="0" t="n">
+      <c r="I26" s="2" t="n">
         <v>0</v>
       </c>
       <c r="M26" s="0" t="n">
@@ -5081,10 +6172,10 @@
       <c r="P26" s="6" t="n">
         <v>4.18</v>
       </c>
-      <c r="Q26" s="7" t="n">
+      <c r="Q26" s="4" t="n">
         <v>266.41</v>
       </c>
-      <c r="R26" s="4" t="n">
+      <c r="R26" s="5" t="n">
         <v>5.4</v>
       </c>
       <c r="S26" s="0" t="n">
@@ -5102,102 +6193,102 @@
       <c r="A27" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="E27" s="3"/>
+      <c r="E27" s="4"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N30" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G31" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="H31" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G31" s="0" t="s">
+      <c r="I31" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H31" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="I31" s="0" t="s">
-        <v>8</v>
-      </c>
       <c r="N31" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="R31" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="S31" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="R31" s="1" t="s">
+      <c r="T31" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="S31" s="0" t="s">
+      <c r="U31" s="0" t="s">
         <v>6</v>
-      </c>
-      <c r="T31" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="U31" s="0" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="C32" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="C32" s="0" t="s">
+      <c r="D32" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D32" s="0" t="s">
+      <c r="E32" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E32" s="0" t="s">
+      <c r="F32" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="G32" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="G32" s="0" t="s">
+      <c r="H32" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="H32" s="0" t="s">
+      <c r="I32" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="I32" s="0" t="s">
-        <v>17</v>
-      </c>
       <c r="M32" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="N32" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="N32" s="0" t="s">
+      <c r="O32" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="O32" s="0" t="s">
+      <c r="P32" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="P32" s="0" t="s">
+      <c r="Q32" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="Q32" s="0" t="s">
+      <c r="R32" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R32" s="1" t="s">
+      <c r="S32" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="S32" s="0" t="s">
+      <c r="T32" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="T32" s="0" t="s">
+      <c r="U32" s="0" t="s">
         <v>16</v>
-      </c>
-      <c r="U32" s="0" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5315,6 +6406,9 @@
       <c r="U34" s="0" t="n">
         <v>0.07</v>
       </c>
+      <c r="AC34" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
@@ -5503,10 +6597,10 @@
       <c r="D38" s="0" t="n">
         <v>0.98</v>
       </c>
-      <c r="E38" s="3" t="n">
+      <c r="E38" s="4" t="n">
         <v>18.65</v>
       </c>
-      <c r="F38" s="4" t="n">
+      <c r="F38" s="5" t="n">
         <v>0.058</v>
       </c>
       <c r="G38" s="0" t="n">
@@ -5531,10 +6625,10 @@
       <c r="P38" s="0" t="n">
         <v>0.97</v>
       </c>
-      <c r="Q38" s="3" t="n">
+      <c r="Q38" s="4" t="n">
         <v>17.05</v>
       </c>
-      <c r="R38" s="4" t="n">
+      <c r="R38" s="5" t="n">
         <v>0.05</v>
       </c>
       <c r="S38" s="0" t="n">
@@ -5561,10 +6655,10 @@
       <c r="D39" s="0" t="n">
         <v>0.98</v>
       </c>
-      <c r="E39" s="3" t="n">
+      <c r="E39" s="4" t="n">
         <v>19.94</v>
       </c>
-      <c r="F39" s="4" t="n">
+      <c r="F39" s="5" t="n">
         <v>0.086</v>
       </c>
       <c r="G39" s="0" t="n">
@@ -5589,10 +6683,10 @@
       <c r="P39" s="0" t="n">
         <v>0.97</v>
       </c>
-      <c r="Q39" s="3" t="n">
+      <c r="Q39" s="4" t="n">
         <v>17.42</v>
       </c>
-      <c r="R39" s="4" t="n">
+      <c r="R39" s="5" t="n">
         <v>0.076</v>
       </c>
       <c r="S39" s="0" t="n">
@@ -5619,10 +6713,10 @@
       <c r="D40" s="0" t="n">
         <v>0.98</v>
       </c>
-      <c r="E40" s="3" t="n">
+      <c r="E40" s="4" t="n">
         <v>20.99</v>
       </c>
-      <c r="F40" s="4" t="n">
+      <c r="F40" s="5" t="n">
         <v>0.117</v>
       </c>
       <c r="G40" s="0" t="n">
@@ -5647,10 +6741,10 @@
       <c r="P40" s="0" t="n">
         <v>0.97</v>
       </c>
-      <c r="Q40" s="3" t="n">
+      <c r="Q40" s="4" t="n">
         <v>18.24</v>
       </c>
-      <c r="R40" s="4" t="n">
+      <c r="R40" s="5" t="n">
         <v>0.107</v>
       </c>
       <c r="S40" s="0" t="n">
@@ -5677,10 +6771,10 @@
       <c r="D41" s="0" t="n">
         <v>0.98</v>
       </c>
-      <c r="E41" s="3" t="n">
+      <c r="E41" s="4" t="n">
         <v>21.73</v>
       </c>
-      <c r="F41" s="4" t="n">
+      <c r="F41" s="5" t="n">
         <v>0.158</v>
       </c>
       <c r="G41" s="0" t="n">
@@ -5705,10 +6799,10 @@
       <c r="P41" s="0" t="n">
         <v>0.97</v>
       </c>
-      <c r="Q41" s="3" t="n">
+      <c r="Q41" s="4" t="n">
         <v>19.1</v>
       </c>
-      <c r="R41" s="4" t="n">
+      <c r="R41" s="5" t="n">
         <v>0.155</v>
       </c>
       <c r="S41" s="0" t="n">
@@ -5735,10 +6829,10 @@
       <c r="D42" s="0" t="n">
         <v>0.97</v>
       </c>
-      <c r="E42" s="3" t="n">
+      <c r="E42" s="4" t="n">
         <v>22.83</v>
       </c>
-      <c r="F42" s="4" t="n">
+      <c r="F42" s="5" t="n">
         <v>0.209</v>
       </c>
       <c r="G42" s="0" t="n">
@@ -5763,10 +6857,10 @@
       <c r="P42" s="0" t="n">
         <v>0.97</v>
       </c>
-      <c r="Q42" s="3" t="n">
+      <c r="Q42" s="4" t="n">
         <v>20.01</v>
       </c>
-      <c r="R42" s="4" t="n">
+      <c r="R42" s="5" t="n">
         <v>0.195</v>
       </c>
       <c r="S42" s="0" t="n">
@@ -5793,10 +6887,10 @@
       <c r="D43" s="0" t="n">
         <v>0.97</v>
       </c>
-      <c r="E43" s="3" t="n">
+      <c r="E43" s="4" t="n">
         <v>23.32</v>
       </c>
-      <c r="F43" s="4" t="n">
+      <c r="F43" s="5" t="n">
         <v>0.27</v>
       </c>
       <c r="G43" s="0" t="n">
@@ -5821,10 +6915,10 @@
       <c r="P43" s="0" t="n">
         <v>0.96</v>
       </c>
-      <c r="Q43" s="3" t="n">
+      <c r="Q43" s="4" t="n">
         <v>20.91</v>
       </c>
-      <c r="R43" s="4" t="n">
+      <c r="R43" s="5" t="n">
         <v>0.268</v>
       </c>
       <c r="S43" s="0" t="n">
@@ -5851,10 +6945,10 @@
       <c r="D44" s="0" t="n">
         <v>0.98</v>
       </c>
-      <c r="E44" s="3" t="n">
+      <c r="E44" s="4" t="n">
         <v>24.95</v>
       </c>
-      <c r="F44" s="4" t="n">
+      <c r="F44" s="5" t="n">
         <v>0.362</v>
       </c>
       <c r="G44" s="0" t="n">
@@ -5879,10 +6973,10 @@
       <c r="P44" s="0" t="n">
         <v>0.95</v>
       </c>
-      <c r="Q44" s="3" t="n">
+      <c r="Q44" s="4" t="n">
         <v>22.36</v>
       </c>
-      <c r="R44" s="4" t="n">
+      <c r="R44" s="5" t="n">
         <v>0.34</v>
       </c>
       <c r="S44" s="0" t="n">
@@ -5909,10 +7003,10 @@
       <c r="D45" s="0" t="n">
         <v>0.97</v>
       </c>
-      <c r="E45" s="3" t="n">
+      <c r="E45" s="4" t="n">
         <v>28.31</v>
       </c>
-      <c r="F45" s="4" t="n">
+      <c r="F45" s="5" t="n">
         <v>0.513</v>
       </c>
       <c r="G45" s="0" t="n">
@@ -5937,10 +7031,10 @@
       <c r="P45" s="0" t="n">
         <v>0.95</v>
       </c>
-      <c r="Q45" s="3" t="n">
+      <c r="Q45" s="4" t="n">
         <v>25.75</v>
       </c>
-      <c r="R45" s="4" t="n">
+      <c r="R45" s="5" t="n">
         <v>0.52</v>
       </c>
       <c r="S45" s="0" t="n">
@@ -5967,10 +7061,10 @@
       <c r="D46" s="0" t="n">
         <v>0.97</v>
       </c>
-      <c r="E46" s="3" t="n">
+      <c r="E46" s="4" t="n">
         <v>33.83</v>
       </c>
-      <c r="F46" s="4" t="n">
+      <c r="F46" s="5" t="n">
         <v>0.754</v>
       </c>
       <c r="G46" s="0" t="n">
@@ -5995,10 +7089,10 @@
       <c r="P46" s="0" t="n">
         <v>0.96</v>
       </c>
-      <c r="Q46" s="3" t="n">
+      <c r="Q46" s="4" t="n">
         <v>29.54</v>
       </c>
-      <c r="R46" s="4" t="n">
+      <c r="R46" s="5" t="n">
         <v>0.715</v>
       </c>
       <c r="S46" s="0" t="n">
@@ -6025,10 +7119,10 @@
       <c r="D47" s="0" t="n">
         <v>0.99</v>
       </c>
-      <c r="E47" s="3" t="n">
+      <c r="E47" s="4" t="n">
         <v>41.93</v>
       </c>
-      <c r="F47" s="4" t="n">
+      <c r="F47" s="5" t="n">
         <v>1.113</v>
       </c>
       <c r="G47" s="0" t="n">
@@ -6053,10 +7147,10 @@
       <c r="P47" s="0" t="n">
         <v>0.96</v>
       </c>
-      <c r="Q47" s="3" t="n">
+      <c r="Q47" s="4" t="n">
         <v>38.19</v>
       </c>
-      <c r="R47" s="4" t="n">
+      <c r="R47" s="5" t="n">
         <v>1.145</v>
       </c>
       <c r="S47" s="0" t="n">
@@ -6074,19 +7168,19 @@
       <c r="A48" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="B48" s="5" t="n">
+      <c r="B48" s="6" t="n">
         <v>64.82</v>
       </c>
-      <c r="C48" s="5" t="n">
+      <c r="C48" s="6" t="n">
         <v>1165.5</v>
       </c>
       <c r="D48" s="6" t="n">
         <v>1.04</v>
       </c>
-      <c r="E48" s="3" t="n">
+      <c r="E48" s="4" t="n">
         <v>54.03</v>
       </c>
-      <c r="F48" s="4" t="n">
+      <c r="F48" s="5" t="n">
         <v>1.612</v>
       </c>
       <c r="G48" s="0" t="n">
@@ -6102,19 +7196,19 @@
       <c r="M48" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="N48" s="5" t="n">
+      <c r="N48" s="6" t="n">
         <v>63.88</v>
       </c>
-      <c r="O48" s="5" t="n">
+      <c r="O48" s="6" t="n">
         <v>1015.9</v>
       </c>
       <c r="P48" s="6" t="n">
         <v>1.01</v>
       </c>
-      <c r="Q48" s="3" t="n">
+      <c r="Q48" s="4" t="n">
         <v>46.49</v>
       </c>
-      <c r="R48" s="4" t="n">
+      <c r="R48" s="5" t="n">
         <v>1.557</v>
       </c>
       <c r="S48" s="0" t="n">
@@ -6141,10 +7235,10 @@
       <c r="D49" s="6" t="n">
         <v>1.12</v>
       </c>
-      <c r="E49" s="3" t="n">
+      <c r="E49" s="4" t="n">
         <v>70.18</v>
       </c>
-      <c r="F49" s="4" t="n">
+      <c r="F49" s="5" t="n">
         <v>2.264</v>
       </c>
       <c r="G49" s="0" t="n">
@@ -6169,10 +7263,10 @@
       <c r="P49" s="6" t="n">
         <v>1.08</v>
       </c>
-      <c r="Q49" s="3" t="n">
+      <c r="Q49" s="4" t="n">
         <v>60.59</v>
       </c>
-      <c r="R49" s="4" t="n">
+      <c r="R49" s="5" t="n">
         <v>2.211</v>
       </c>
       <c r="S49" s="0" t="n">
@@ -6199,10 +7293,10 @@
       <c r="D50" s="6" t="n">
         <v>1.27</v>
       </c>
-      <c r="E50" s="3" t="n">
+      <c r="E50" s="4" t="n">
         <v>90.55</v>
       </c>
-      <c r="F50" s="4" t="n">
+      <c r="F50" s="5" t="n">
         <v>3.06</v>
       </c>
       <c r="G50" s="0" t="n">
@@ -6227,10 +7321,10 @@
       <c r="P50" s="6" t="n">
         <v>1.27</v>
       </c>
-      <c r="Q50" s="3" t="n">
+      <c r="Q50" s="4" t="n">
         <v>91.12</v>
       </c>
-      <c r="R50" s="4" t="n">
+      <c r="R50" s="5" t="n">
         <v>3.172</v>
       </c>
       <c r="S50" s="0" t="n">
@@ -6257,10 +7351,10 @@
       <c r="D51" s="6" t="n">
         <v>1.49</v>
       </c>
-      <c r="E51" s="3" t="n">
+      <c r="E51" s="4" t="n">
         <v>115.61</v>
       </c>
-      <c r="F51" s="4" t="n">
+      <c r="F51" s="5" t="n">
         <v>3.981</v>
       </c>
       <c r="G51" s="0" t="n">
@@ -6285,10 +7379,10 @@
       <c r="P51" s="6" t="n">
         <v>1.48</v>
       </c>
-      <c r="Q51" s="3" t="n">
+      <c r="Q51" s="4" t="n">
         <v>102.61</v>
       </c>
-      <c r="R51" s="4" t="n">
+      <c r="R51" s="5" t="n">
         <v>3.944</v>
       </c>
       <c r="S51" s="0" t="n">
@@ -6315,10 +7409,10 @@
       <c r="D52" s="6" t="n">
         <v>1.83</v>
       </c>
-      <c r="E52" s="3" t="n">
+      <c r="E52" s="4" t="n">
         <v>147.67</v>
       </c>
-      <c r="F52" s="4" t="n">
+      <c r="F52" s="5" t="n">
         <v>5.02</v>
       </c>
       <c r="G52" s="0" t="n">
@@ -6343,10 +7437,10 @@
       <c r="P52" s="6" t="n">
         <v>1.94</v>
       </c>
-      <c r="Q52" s="3" t="n">
+      <c r="Q52" s="4" t="n">
         <v>138.17</v>
       </c>
-      <c r="R52" s="4" t="n">
+      <c r="R52" s="5" t="n">
         <v>5.142</v>
       </c>
       <c r="S52" s="0" t="n">
@@ -6373,10 +7467,10 @@
       <c r="D53" s="6" t="n">
         <v>2.31</v>
       </c>
-      <c r="E53" s="3" t="n">
+      <c r="E53" s="4" t="n">
         <v>188.19</v>
       </c>
-      <c r="F53" s="4" t="n">
+      <c r="F53" s="5" t="n">
         <v>6.1</v>
       </c>
       <c r="G53" s="0" t="n">
@@ -6401,10 +7495,10 @@
       <c r="P53" s="6" t="n">
         <v>2.5</v>
       </c>
-      <c r="Q53" s="3" t="n">
+      <c r="Q53" s="4" t="n">
         <v>176.37</v>
       </c>
-      <c r="R53" s="4" t="n">
+      <c r="R53" s="5" t="n">
         <v>6.036</v>
       </c>
       <c r="S53" s="0" t="n">
@@ -6417,6 +7511,9 @@
       <c r="U53" s="0" t="n">
         <v>444.3</v>
       </c>
+      <c r="AC53" s="0" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="n">
@@ -6431,10 +7528,10 @@
       <c r="D54" s="6" t="n">
         <v>3.37</v>
       </c>
-      <c r="E54" s="7" t="n">
+      <c r="E54" s="4" t="n">
         <v>261.2</v>
       </c>
-      <c r="F54" s="4" t="n">
+      <c r="F54" s="5" t="n">
         <v>5.4</v>
       </c>
       <c r="G54" s="0" t="n">
@@ -6459,10 +7556,10 @@
       <c r="P54" s="6" t="n">
         <v>4.06</v>
       </c>
-      <c r="Q54" s="7" t="n">
+      <c r="Q54" s="4" t="n">
         <v>255.62</v>
       </c>
-      <c r="R54" s="4" t="n">
+      <c r="R54" s="5" t="n">
         <v>5.5</v>
       </c>
       <c r="S54" s="0" t="n">
@@ -6472,100 +7569,103 @@
         <v>0</v>
       </c>
     </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="N59" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G60" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F60" s="1" t="s">
+      <c r="H60" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G60" s="0" t="s">
+      <c r="I60" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H60" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="I60" s="0" t="s">
-        <v>8</v>
-      </c>
       <c r="N60" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="R60" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="S60" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="R60" s="1" t="s">
+      <c r="T60" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="S60" s="0" t="s">
+      <c r="U60" s="0" t="s">
         <v>6</v>
-      </c>
-      <c r="T60" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="U60" s="0" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B61" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B61" s="0" t="s">
+      <c r="C61" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="C61" s="0" t="s">
+      <c r="D61" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D61" s="0" t="s">
+      <c r="E61" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E61" s="0" t="s">
+      <c r="F61" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F61" s="1" t="s">
+      <c r="G61" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="G61" s="0" t="s">
+      <c r="H61" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="H61" s="0" t="s">
+      <c r="I61" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="I61" s="0" t="s">
-        <v>17</v>
-      </c>
       <c r="M61" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="N61" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="N61" s="0" t="s">
+      <c r="O61" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="O61" s="0" t="s">
+      <c r="P61" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="P61" s="0" t="s">
+      <c r="Q61" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="Q61" s="0" t="s">
+      <c r="R61" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R61" s="1" t="s">
+      <c r="S61" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="S61" s="0" t="s">
+      <c r="T61" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="T61" s="0" t="s">
+      <c r="U61" s="0" t="s">
         <v>16</v>
-      </c>
-      <c r="U61" s="0" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6871,10 +7971,10 @@
       <c r="D67" s="0" t="n">
         <v>0.96</v>
       </c>
-      <c r="E67" s="3" t="n">
+      <c r="E67" s="4" t="n">
         <v>15.51</v>
       </c>
-      <c r="F67" s="4" t="n">
+      <c r="F67" s="5" t="n">
         <v>0.046</v>
       </c>
       <c r="G67" s="0" t="n">
@@ -6899,10 +7999,10 @@
       <c r="P67" s="0" t="n">
         <v>0.95</v>
       </c>
-      <c r="Q67" s="3" t="n">
+      <c r="Q67" s="4" t="n">
         <v>14.17</v>
       </c>
-      <c r="R67" s="4" t="n">
+      <c r="R67" s="5" t="n">
         <v>0.04</v>
       </c>
       <c r="S67" s="0" t="n">
@@ -6929,10 +8029,10 @@
       <c r="D68" s="0" t="n">
         <v>0.94</v>
       </c>
-      <c r="E68" s="3" t="n">
+      <c r="E68" s="4" t="n">
         <v>16.31</v>
       </c>
-      <c r="F68" s="4" t="n">
+      <c r="F68" s="5" t="n">
         <v>0.08</v>
       </c>
       <c r="G68" s="0" t="n">
@@ -6957,10 +8057,10 @@
       <c r="P68" s="0" t="n">
         <v>0.93</v>
       </c>
-      <c r="Q68" s="3" t="n">
+      <c r="Q68" s="4" t="n">
         <v>14.38</v>
       </c>
-      <c r="R68" s="4" t="n">
+      <c r="R68" s="5" t="n">
         <v>0.06</v>
       </c>
       <c r="S68" s="0" t="n">
@@ -6987,10 +8087,10 @@
       <c r="D69" s="0" t="n">
         <v>0.96</v>
       </c>
-      <c r="E69" s="3" t="n">
+      <c r="E69" s="4" t="n">
         <v>16.42</v>
       </c>
-      <c r="F69" s="4" t="n">
+      <c r="F69" s="5" t="n">
         <v>0.104</v>
       </c>
       <c r="G69" s="0" t="n">
@@ -7015,10 +8115,10 @@
       <c r="P69" s="0" t="n">
         <v>0.94</v>
       </c>
-      <c r="Q69" s="3" t="n">
+      <c r="Q69" s="4" t="n">
         <v>14.79</v>
       </c>
-      <c r="R69" s="4" t="n">
+      <c r="R69" s="5" t="n">
         <v>0.1</v>
       </c>
       <c r="S69" s="0" t="n">
@@ -7045,10 +8145,10 @@
       <c r="D70" s="0" t="n">
         <v>0.96</v>
       </c>
-      <c r="E70" s="3" t="n">
+      <c r="E70" s="4" t="n">
         <v>17.18</v>
       </c>
-      <c r="F70" s="4" t="n">
+      <c r="F70" s="5" t="n">
         <v>0.148</v>
       </c>
       <c r="G70" s="0" t="n">
@@ -7073,10 +8173,10 @@
       <c r="P70" s="0" t="n">
         <v>0.93</v>
       </c>
-      <c r="Q70" s="3" t="n">
+      <c r="Q70" s="4" t="n">
         <v>15.24</v>
       </c>
-      <c r="R70" s="4" t="n">
+      <c r="R70" s="5" t="n">
         <v>0.13</v>
       </c>
       <c r="S70" s="0" t="n">
@@ -7103,10 +8203,10 @@
       <c r="D71" s="0" t="n">
         <v>0.95</v>
       </c>
-      <c r="E71" s="3" t="n">
+      <c r="E71" s="4" t="n">
         <v>18.42</v>
       </c>
-      <c r="F71" s="4" t="n">
+      <c r="F71" s="5" t="n">
         <v>0.18</v>
       </c>
       <c r="G71" s="0" t="n">
@@ -7131,10 +8231,10 @@
       <c r="P71" s="0" t="n">
         <v>0.92</v>
       </c>
-      <c r="Q71" s="3" t="n">
+      <c r="Q71" s="4" t="n">
         <v>15.51</v>
       </c>
-      <c r="R71" s="4" t="n">
+      <c r="R71" s="5" t="n">
         <v>0.17</v>
       </c>
       <c r="S71" s="0" t="n">
@@ -7161,10 +8261,10 @@
       <c r="D72" s="0" t="n">
         <v>0.95</v>
       </c>
-      <c r="E72" s="3" t="n">
+      <c r="E72" s="4" t="n">
         <v>19.96</v>
       </c>
-      <c r="F72" s="4" t="n">
+      <c r="F72" s="5" t="n">
         <v>0.24</v>
       </c>
       <c r="G72" s="0" t="n">
@@ -7189,10 +8289,10 @@
       <c r="P72" s="0" t="n">
         <v>0.93</v>
       </c>
-      <c r="Q72" s="3" t="n">
+      <c r="Q72" s="4" t="n">
         <v>16.66</v>
       </c>
-      <c r="R72" s="4" t="n">
+      <c r="R72" s="5" t="n">
         <v>0.23</v>
       </c>
       <c r="S72" s="0" t="n">
@@ -7219,10 +8319,10 @@
       <c r="D73" s="0" t="n">
         <v>0.94</v>
       </c>
-      <c r="E73" s="3" t="n">
+      <c r="E73" s="4" t="n">
         <v>20.51</v>
       </c>
-      <c r="F73" s="4" t="n">
+      <c r="F73" s="5" t="n">
         <v>0.33</v>
       </c>
       <c r="G73" s="0" t="n">
@@ -7247,10 +8347,10 @@
       <c r="P73" s="0" t="n">
         <v>0.92</v>
       </c>
-      <c r="Q73" s="3" t="n">
+      <c r="Q73" s="4" t="n">
         <v>17.13</v>
       </c>
-      <c r="R73" s="4" t="n">
+      <c r="R73" s="5" t="n">
         <v>0.31</v>
       </c>
       <c r="S73" s="0" t="n">
@@ -7277,10 +8377,10 @@
       <c r="D74" s="0" t="n">
         <v>0.93</v>
       </c>
-      <c r="E74" s="3" t="n">
+      <c r="E74" s="4" t="n">
         <v>21.88</v>
       </c>
-      <c r="F74" s="4" t="n">
+      <c r="F74" s="5" t="n">
         <v>0.48</v>
       </c>
       <c r="G74" s="0" t="n">
@@ -7305,10 +8405,10 @@
       <c r="P74" s="0" t="n">
         <v>0.92</v>
       </c>
-      <c r="Q74" s="3" t="n">
+      <c r="Q74" s="4" t="n">
         <v>19.16</v>
       </c>
-      <c r="R74" s="4" t="n">
+      <c r="R74" s="5" t="n">
         <v>0.46</v>
       </c>
       <c r="S74" s="0" t="n">
@@ -7335,10 +8435,10 @@
       <c r="D75" s="0" t="n">
         <v>0.94</v>
       </c>
-      <c r="E75" s="3" t="n">
+      <c r="E75" s="4" t="n">
         <v>26.05</v>
       </c>
-      <c r="F75" s="4" t="n">
+      <c r="F75" s="5" t="n">
         <v>0.7</v>
       </c>
       <c r="G75" s="0" t="n">
@@ -7363,10 +8463,10 @@
       <c r="P75" s="0" t="n">
         <v>0.91</v>
       </c>
-      <c r="Q75" s="3" t="n">
+      <c r="Q75" s="4" t="n">
         <v>22.86</v>
       </c>
-      <c r="R75" s="4" t="n">
+      <c r="R75" s="5" t="n">
         <v>0.7</v>
       </c>
       <c r="S75" s="0" t="n">
@@ -7393,10 +8493,10 @@
       <c r="D76" s="0" t="n">
         <v>0.94</v>
       </c>
-      <c r="E76" s="3" t="n">
+      <c r="E76" s="4" t="n">
         <v>32.04</v>
       </c>
-      <c r="F76" s="4" t="n">
+      <c r="F76" s="5" t="n">
         <v>1.07</v>
       </c>
       <c r="G76" s="0" t="n">
@@ -7421,10 +8521,10 @@
       <c r="P76" s="0" t="n">
         <v>0.91</v>
       </c>
-      <c r="Q76" s="3" t="n">
+      <c r="Q76" s="4" t="n">
         <v>26.79</v>
       </c>
-      <c r="R76" s="4" t="n">
+      <c r="R76" s="5" t="n">
         <v>1.05</v>
       </c>
       <c r="S76" s="0" t="n">
@@ -7442,19 +8542,19 @@
       <c r="A77" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="B77" s="5" t="n">
+      <c r="B77" s="6" t="n">
         <v>65.73</v>
       </c>
-      <c r="C77" s="5" t="n">
+      <c r="C77" s="6" t="n">
         <v>864.9</v>
       </c>
       <c r="D77" s="6" t="n">
         <v>0.98</v>
       </c>
-      <c r="E77" s="3" t="n">
+      <c r="E77" s="4" t="n">
         <v>40.82</v>
       </c>
-      <c r="F77" s="4" t="n">
+      <c r="F77" s="5" t="n">
         <v>1.57</v>
       </c>
       <c r="G77" s="0" t="n">
@@ -7470,19 +8570,19 @@
       <c r="M77" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="N77" s="5" t="n">
+      <c r="N77" s="6" t="n">
         <v>67.36</v>
       </c>
-      <c r="O77" s="5" t="n">
+      <c r="O77" s="6" t="n">
         <v>714.3</v>
       </c>
       <c r="P77" s="6" t="n">
         <v>0.94</v>
       </c>
-      <c r="Q77" s="3" t="n">
+      <c r="Q77" s="4" t="n">
         <v>24.6</v>
       </c>
-      <c r="R77" s="4" t="n">
+      <c r="R77" s="5" t="n">
         <v>1.54</v>
       </c>
       <c r="S77" s="0" t="n">
@@ -7509,10 +8609,10 @@
       <c r="D78" s="6" t="n">
         <v>1.08</v>
       </c>
-      <c r="E78" s="3" t="n">
+      <c r="E78" s="4" t="n">
         <v>53.75</v>
       </c>
-      <c r="F78" s="4" t="n">
+      <c r="F78" s="5" t="n">
         <v>2.2</v>
       </c>
       <c r="G78" s="0" t="n">
@@ -7537,10 +8637,10 @@
       <c r="P78" s="6" t="n">
         <v>1.05</v>
       </c>
-      <c r="Q78" s="3" t="n">
+      <c r="Q78" s="4" t="n">
         <v>44.7</v>
       </c>
-      <c r="R78" s="4" t="n">
+      <c r="R78" s="5" t="n">
         <v>2.2</v>
       </c>
       <c r="S78" s="0" t="n">
@@ -7567,10 +8667,10 @@
       <c r="D79" s="6" t="n">
         <v>1.23</v>
       </c>
-      <c r="E79" s="3" t="n">
+      <c r="E79" s="4" t="n">
         <v>69.12</v>
       </c>
-      <c r="F79" s="4" t="n">
+      <c r="F79" s="5" t="n">
         <v>3</v>
       </c>
       <c r="G79" s="0" t="n">
@@ -7595,10 +8695,10 @@
       <c r="P79" s="6" t="n">
         <v>1.23</v>
       </c>
-      <c r="Q79" s="3" t="n">
+      <c r="Q79" s="4" t="n">
         <v>58.43</v>
       </c>
-      <c r="R79" s="4" t="n">
+      <c r="R79" s="5" t="n">
         <v>2.99</v>
       </c>
       <c r="S79" s="0" t="n">
@@ -7625,10 +8725,10 @@
       <c r="D80" s="6" t="n">
         <v>1.57</v>
       </c>
-      <c r="E80" s="3" t="n">
+      <c r="E80" s="4" t="n">
         <v>74.45</v>
       </c>
-      <c r="F80" s="4" t="n">
+      <c r="F80" s="5" t="n">
         <v>4.1</v>
       </c>
       <c r="G80" s="0" t="n">
@@ -7653,10 +8753,10 @@
       <c r="P80" s="6" t="n">
         <v>1.54</v>
       </c>
-      <c r="Q80" s="3" t="n">
+      <c r="Q80" s="4" t="n">
         <v>77.54</v>
       </c>
-      <c r="R80" s="4" t="n">
+      <c r="R80" s="5" t="n">
         <v>3.9</v>
       </c>
       <c r="S80" s="0" t="n">
@@ -7683,10 +8783,10 @@
       <c r="D81" s="6" t="n">
         <v>1.96</v>
       </c>
-      <c r="E81" s="3" t="n">
+      <c r="E81" s="4" t="n">
         <v>119.27</v>
       </c>
-      <c r="F81" s="4" t="n">
+      <c r="F81" s="5" t="n">
         <v>4.9</v>
       </c>
       <c r="G81" s="0" t="n">
@@ -7711,10 +8811,10 @@
       <c r="P81" s="6" t="n">
         <v>2.33</v>
       </c>
-      <c r="Q81" s="3" t="n">
+      <c r="Q81" s="4" t="n">
         <v>113.32</v>
       </c>
-      <c r="R81" s="4" t="n">
+      <c r="R81" s="5" t="n">
         <v>4.88</v>
       </c>
       <c r="S81" s="0" t="n">
@@ -7741,10 +8841,10 @@
       <c r="D82" s="6" t="n">
         <v>3.66</v>
       </c>
-      <c r="E82" s="3" t="n">
+      <c r="E82" s="4" t="n">
         <v>196.84</v>
       </c>
-      <c r="F82" s="4" t="n">
+      <c r="F82" s="5" t="n">
         <v>5.3</v>
       </c>
       <c r="G82" s="0" t="n">
@@ -7769,10 +8869,10 @@
       <c r="P82" s="6" t="n">
         <v>3.18</v>
       </c>
-      <c r="Q82" s="3" t="n">
+      <c r="Q82" s="4" t="n">
         <v>142.16</v>
       </c>
-      <c r="R82" s="4" t="n">
+      <c r="R82" s="5" t="n">
         <v>4.5</v>
       </c>
       <c r="S82" s="0" t="n">
@@ -7787,98 +8887,98 @@
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="N88" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G89" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F89" s="1" t="s">
+      <c r="H89" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G89" s="0" t="s">
+      <c r="I89" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H89" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="I89" s="0" t="s">
-        <v>8</v>
-      </c>
       <c r="N89" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="R89" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="S89" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="R89" s="1" t="s">
+      <c r="T89" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="S89" s="0" t="s">
+      <c r="U89" s="0" t="s">
         <v>6</v>
-      </c>
-      <c r="T89" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="U89" s="0" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B90" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B90" s="0" t="s">
+      <c r="C90" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="C90" s="0" t="s">
+      <c r="D90" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D90" s="0" t="s">
+      <c r="E90" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E90" s="0" t="s">
+      <c r="F90" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F90" s="1" t="s">
+      <c r="G90" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="G90" s="0" t="s">
+      <c r="H90" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="H90" s="0" t="s">
+      <c r="I90" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="I90" s="0" t="s">
-        <v>17</v>
-      </c>
       <c r="M90" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="N90" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="N90" s="0" t="s">
+      <c r="O90" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="O90" s="0" t="s">
+      <c r="P90" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="P90" s="0" t="s">
+      <c r="Q90" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="Q90" s="0" t="s">
+      <c r="R90" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R90" s="1" t="s">
+      <c r="S90" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="S90" s="0" t="s">
+      <c r="T90" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="T90" s="0" t="s">
+      <c r="U90" s="0" t="s">
         <v>16</v>
-      </c>
-      <c r="U90" s="0" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8154,10 +9254,10 @@
       <c r="P95" s="0" t="n">
         <v>0.77</v>
       </c>
-      <c r="Q95" s="3" t="n">
+      <c r="Q95" s="4" t="n">
         <v>7.67</v>
       </c>
-      <c r="R95" s="4" t="n">
+      <c r="R95" s="5" t="n">
         <v>0.008</v>
       </c>
       <c r="S95" s="0" t="n">
@@ -8184,10 +9284,10 @@
       <c r="D96" s="0" t="n">
         <v>0.91</v>
       </c>
-      <c r="E96" s="3" t="n">
+      <c r="E96" s="4" t="n">
         <v>12.53</v>
       </c>
-      <c r="F96" s="4" t="n">
+      <c r="F96" s="5" t="n">
         <v>0.036</v>
       </c>
       <c r="G96" s="0" t="n">
@@ -8212,10 +9312,10 @@
       <c r="P96" s="0" t="n">
         <v>0.78</v>
       </c>
-      <c r="Q96" s="3" t="n">
+      <c r="Q96" s="4" t="n">
         <v>7.82</v>
       </c>
-      <c r="R96" s="4" t="n">
+      <c r="R96" s="5" t="n">
         <v>0.02</v>
       </c>
       <c r="S96" s="0" t="n">
@@ -8242,10 +9342,10 @@
       <c r="D97" s="0" t="n">
         <v>0.9</v>
       </c>
-      <c r="E97" s="3" t="n">
+      <c r="E97" s="4" t="n">
         <v>12.48</v>
       </c>
-      <c r="F97" s="4" t="n">
+      <c r="F97" s="5" t="n">
         <v>0.058</v>
       </c>
       <c r="G97" s="0" t="n">
@@ -8270,10 +9370,10 @@
       <c r="P97" s="0" t="n">
         <v>0.77</v>
       </c>
-      <c r="Q97" s="3" t="n">
+      <c r="Q97" s="4" t="n">
         <v>7.83</v>
       </c>
-      <c r="R97" s="4" t="n">
+      <c r="R97" s="5" t="n">
         <v>0.04</v>
       </c>
       <c r="S97" s="0" t="n">
@@ -8300,10 +9400,10 @@
       <c r="D98" s="0" t="n">
         <v>0.91</v>
       </c>
-      <c r="E98" s="3" t="n">
+      <c r="E98" s="4" t="n">
         <v>12.91</v>
       </c>
-      <c r="F98" s="4" t="n">
+      <c r="F98" s="5" t="n">
         <v>0.085</v>
       </c>
       <c r="G98" s="0" t="n">
@@ -8328,10 +9428,10 @@
       <c r="P98" s="0" t="n">
         <v>0.77</v>
       </c>
-      <c r="Q98" s="3" t="n">
+      <c r="Q98" s="4" t="n">
         <v>7.88</v>
       </c>
-      <c r="R98" s="4" t="n">
+      <c r="R98" s="5" t="n">
         <v>0.065</v>
       </c>
       <c r="S98" s="0" t="n">
@@ -8358,10 +9458,10 @@
       <c r="D99" s="0" t="n">
         <v>0.91</v>
       </c>
-      <c r="E99" s="3" t="n">
+      <c r="E99" s="4" t="n">
         <v>12.98</v>
       </c>
-      <c r="F99" s="4" t="n">
+      <c r="F99" s="5" t="n">
         <v>0.12</v>
       </c>
       <c r="G99" s="0" t="n">
@@ -8386,10 +9486,10 @@
       <c r="P99" s="0" t="n">
         <v>0.78</v>
       </c>
-      <c r="Q99" s="3" t="n">
+      <c r="Q99" s="4" t="n">
         <v>7.98</v>
       </c>
-      <c r="R99" s="4" t="n">
+      <c r="R99" s="5" t="n">
         <v>0.1</v>
       </c>
       <c r="S99" s="0" t="n">
@@ -8416,10 +9516,10 @@
       <c r="D100" s="0" t="n">
         <v>0.9</v>
       </c>
-      <c r="E100" s="3" t="n">
+      <c r="E100" s="4" t="n">
         <v>13.33</v>
       </c>
-      <c r="F100" s="4" t="n">
+      <c r="F100" s="5" t="n">
         <v>0.162</v>
       </c>
       <c r="G100" s="0" t="n">
@@ -8444,10 +9544,10 @@
       <c r="P100" s="0" t="n">
         <v>0.78</v>
       </c>
-      <c r="Q100" s="3" t="n">
+      <c r="Q100" s="4" t="n">
         <v>8.08</v>
       </c>
-      <c r="R100" s="4" t="n">
+      <c r="R100" s="5" t="n">
         <v>0.134</v>
       </c>
       <c r="S100" s="0" t="n">
@@ -8474,10 +9574,10 @@
       <c r="D101" s="0" t="n">
         <v>0.89</v>
       </c>
-      <c r="E101" s="3" t="n">
+      <c r="E101" s="4" t="n">
         <v>13.94</v>
       </c>
-      <c r="F101" s="4" t="n">
+      <c r="F101" s="5" t="n">
         <v>0.215</v>
       </c>
       <c r="G101" s="0" t="n">
@@ -8502,10 +9602,10 @@
       <c r="P101" s="0" t="n">
         <v>0.76</v>
       </c>
-      <c r="Q101" s="3" t="n">
+      <c r="Q101" s="4" t="n">
         <v>8.25</v>
       </c>
-      <c r="R101" s="4" t="n">
+      <c r="R101" s="5" t="n">
         <v>0.189</v>
       </c>
       <c r="S101" s="0" t="n">
@@ -8532,10 +9632,10 @@
       <c r="D102" s="0" t="n">
         <v>0.89</v>
       </c>
-      <c r="E102" s="3" t="n">
+      <c r="E102" s="4" t="n">
         <v>14.61</v>
       </c>
-      <c r="F102" s="4" t="n">
+      <c r="F102" s="5" t="n">
         <v>0.295</v>
       </c>
       <c r="G102" s="0" t="n">
@@ -8560,10 +9660,10 @@
       <c r="P102" s="0" t="n">
         <v>0.75</v>
       </c>
-      <c r="Q102" s="3" t="n">
+      <c r="Q102" s="4" t="n">
         <v>8.54</v>
       </c>
-      <c r="R102" s="4" t="n">
+      <c r="R102" s="5" t="n">
         <v>0.262</v>
       </c>
       <c r="S102" s="0" t="n">
@@ -8590,10 +9690,10 @@
       <c r="D103" s="0" t="n">
         <v>0.88</v>
       </c>
-      <c r="E103" s="3" t="n">
+      <c r="E103" s="4" t="n">
         <v>16.02</v>
       </c>
-      <c r="F103" s="4" t="n">
+      <c r="F103" s="5" t="n">
         <v>0.432</v>
       </c>
       <c r="G103" s="0" t="n">
@@ -8618,10 +9718,10 @@
       <c r="P103" s="0" t="n">
         <v>0.74</v>
       </c>
-      <c r="Q103" s="3" t="n">
+      <c r="Q103" s="4" t="n">
         <v>9.06</v>
       </c>
-      <c r="R103" s="4" t="n">
+      <c r="R103" s="5" t="n">
         <v>0.39</v>
       </c>
       <c r="S103" s="0" t="n">
@@ -8648,10 +9748,10 @@
       <c r="D104" s="0" t="n">
         <v>0.88</v>
       </c>
-      <c r="E104" s="3" t="n">
+      <c r="E104" s="4" t="n">
         <v>18.05</v>
       </c>
-      <c r="F104" s="4" t="n">
+      <c r="F104" s="5" t="n">
         <v>0.655</v>
       </c>
       <c r="G104" s="0" t="n">
@@ -8676,10 +9776,10 @@
       <c r="P104" s="0" t="n">
         <v>0.72</v>
       </c>
-      <c r="Q104" s="3" t="n">
+      <c r="Q104" s="4" t="n">
         <v>9.94</v>
       </c>
-      <c r="R104" s="4" t="n">
+      <c r="R104" s="5" t="n">
         <v>0.61</v>
       </c>
       <c r="S104" s="0" t="n">
@@ -8706,10 +9806,10 @@
       <c r="D105" s="0" t="n">
         <v>0.88</v>
       </c>
-      <c r="E105" s="3" t="n">
+      <c r="E105" s="4" t="n">
         <v>21.7</v>
       </c>
-      <c r="F105" s="4" t="n">
+      <c r="F105" s="5" t="n">
         <v>0.998</v>
       </c>
       <c r="G105" s="0" t="n">
@@ -8734,10 +9834,10 @@
       <c r="P105" s="0" t="n">
         <v>0.72</v>
       </c>
-      <c r="Q105" s="3" t="n">
+      <c r="Q105" s="4" t="n">
         <v>11.51</v>
       </c>
-      <c r="R105" s="4" t="n">
+      <c r="R105" s="5" t="n">
         <v>0.95</v>
       </c>
       <c r="S105" s="0" t="n">
@@ -8755,19 +9855,19 @@
       <c r="A106" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="B106" s="5" t="n">
+      <c r="B106" s="6" t="n">
         <v>67.58</v>
       </c>
-      <c r="C106" s="5" t="n">
+      <c r="C106" s="6" t="n">
         <v>564</v>
       </c>
       <c r="D106" s="6" t="n">
         <v>0.91</v>
       </c>
-      <c r="E106" s="3" t="n">
+      <c r="E106" s="4" t="n">
         <v>27.43</v>
       </c>
-      <c r="F106" s="4" t="n">
+      <c r="F106" s="5" t="n">
         <v>1.49</v>
       </c>
       <c r="G106" s="0" t="n">
@@ -8783,19 +9883,19 @@
       <c r="M106" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="N106" s="5" t="n">
+      <c r="N106" s="6" t="n">
         <v>78.33</v>
       </c>
-      <c r="O106" s="5" t="n">
+      <c r="O106" s="6" t="n">
         <v>258.2</v>
       </c>
       <c r="P106" s="6" t="n">
         <v>0.79</v>
       </c>
-      <c r="Q106" s="3" t="n">
+      <c r="Q106" s="4" t="n">
         <v>14.34</v>
       </c>
-      <c r="R106" s="4" t="n">
+      <c r="R106" s="5" t="n">
         <v>1.43</v>
       </c>
       <c r="S106" s="0" t="n">
@@ -8822,10 +9922,10 @@
       <c r="D107" s="6" t="n">
         <v>1.01</v>
       </c>
-      <c r="E107" s="3" t="n">
+      <c r="E107" s="4" t="n">
         <v>35.79</v>
       </c>
-      <c r="F107" s="4" t="n">
+      <c r="F107" s="5" t="n">
         <v>2.132</v>
       </c>
       <c r="G107" s="0" t="n">
@@ -8850,10 +9950,10 @@
       <c r="P107" s="6" t="n">
         <v>1.38</v>
       </c>
-      <c r="Q107" s="3" t="n">
+      <c r="Q107" s="4" t="n">
         <v>24.72</v>
       </c>
-      <c r="R107" s="4" t="n">
+      <c r="R107" s="5" t="n">
         <v>2</v>
       </c>
       <c r="S107" s="0" t="n">
@@ -8880,10 +9980,10 @@
       <c r="D108" s="6" t="n">
         <v>1.22</v>
       </c>
-      <c r="E108" s="3" t="n">
+      <c r="E108" s="4" t="n">
         <v>47.84</v>
       </c>
-      <c r="F108" s="4" t="n">
+      <c r="F108" s="5" t="n">
         <v>3.046</v>
       </c>
       <c r="G108" s="0" t="n">
@@ -8899,10 +9999,10 @@
       <c r="M108" s="0" t="n">
         <v>34</v>
       </c>
-      <c r="N108" s="5"/>
-      <c r="O108" s="5"/>
-      <c r="P108" s="5"/>
-      <c r="Q108" s="3"/>
+      <c r="N108" s="6"/>
+      <c r="O108" s="6"/>
+      <c r="P108" s="6"/>
+      <c r="Q108" s="4"/>
       <c r="T108" s="0" t="n">
         <f aca="false">P108</f>
         <v>0</v>
@@ -8921,10 +10021,10 @@
       <c r="D109" s="6" t="n">
         <v>1.69</v>
       </c>
-      <c r="E109" s="3" t="n">
+      <c r="E109" s="4" t="n">
         <v>66.67</v>
       </c>
-      <c r="F109" s="4" t="n">
+      <c r="F109" s="5" t="n">
         <v>3.816</v>
       </c>
       <c r="G109" s="0" t="n">
@@ -8940,10 +10040,10 @@
       <c r="M109" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="N109" s="5"/>
-      <c r="O109" s="5"/>
-      <c r="P109" s="5"/>
-      <c r="Q109" s="3"/>
+      <c r="N109" s="6"/>
+      <c r="O109" s="6"/>
+      <c r="P109" s="6"/>
+      <c r="Q109" s="4"/>
       <c r="T109" s="0" t="n">
         <f aca="false">P109</f>
         <v>0</v>
@@ -8962,10 +10062,10 @@
       <c r="D110" s="6" t="n">
         <v>2.64</v>
       </c>
-      <c r="E110" s="3" t="n">
+      <c r="E110" s="4" t="n">
         <v>94.24</v>
       </c>
-      <c r="F110" s="4" t="n">
+      <c r="F110" s="5" t="n">
         <v>4.8</v>
       </c>
       <c r="G110" s="0" t="n">
@@ -8981,10 +10081,10 @@
       <c r="M110" s="0" t="n">
         <v>38</v>
       </c>
-      <c r="N110" s="5"/>
-      <c r="O110" s="5"/>
-      <c r="P110" s="5"/>
-      <c r="Q110" s="3"/>
+      <c r="N110" s="6"/>
+      <c r="O110" s="6"/>
+      <c r="P110" s="6"/>
+      <c r="Q110" s="4"/>
       <c r="T110" s="0" t="n">
         <f aca="false">P110</f>
         <v>0</v>
@@ -8994,10 +10094,10 @@
       <c r="A111" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="B111" s="5"/>
-      <c r="C111" s="5"/>
-      <c r="D111" s="5"/>
-      <c r="E111" s="3"/>
+      <c r="B111" s="6"/>
+      <c r="C111" s="6"/>
+      <c r="D111" s="6"/>
+      <c r="E111" s="4"/>
       <c r="G111" s="0" t="n">
         <v>0</v>
       </c>
@@ -9011,10 +10111,10 @@
       <c r="M111" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="N111" s="5"/>
-      <c r="O111" s="5"/>
-      <c r="P111" s="5"/>
-      <c r="Q111" s="3"/>
+      <c r="N111" s="6"/>
+      <c r="O111" s="6"/>
+      <c r="P111" s="6"/>
+      <c r="Q111" s="4"/>
       <c r="T111" s="0" t="n">
         <f aca="false">P111</f>
         <v>0</v>
@@ -9061,71 +10161,71 @@
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="H3" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="I3" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>8</v>
-      </c>
       <c r="L3" s="0" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="U3" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="E4" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="0" t="s">
-        <v>13</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="G4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="I4" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="0" t="s">
-        <v>17</v>
-      </c>
       <c r="K4" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="P4" s="1"/>
-      <c r="U4" s="2"/>
+      <c r="U4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -9136,7 +10236,7 @@
         <v>0</v>
       </c>
       <c r="P5" s="1"/>
-      <c r="U5" s="2"/>
+      <c r="U5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -9147,7 +10247,7 @@
         <v>5</v>
       </c>
       <c r="P6" s="1"/>
-      <c r="U6" s="2"/>
+      <c r="U6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -9158,7 +10258,7 @@
         <v>10</v>
       </c>
       <c r="P7" s="1"/>
-      <c r="U7" s="2"/>
+      <c r="U7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -9169,7 +10269,7 @@
         <v>15</v>
       </c>
       <c r="P8" s="1"/>
-      <c r="U8" s="2"/>
+      <c r="U8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
@@ -9180,18 +10280,18 @@
         <v>20</v>
       </c>
       <c r="P9" s="1"/>
-      <c r="U9" s="2"/>
+      <c r="U9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="F10" s="4"/>
+      <c r="F10" s="5"/>
       <c r="K10" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="P10" s="4"/>
-      <c r="U10" s="2"/>
+      <c r="P10" s="5"/>
+      <c r="U10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
@@ -9202,7 +10302,7 @@
         <v>30</v>
       </c>
       <c r="P11" s="1"/>
-      <c r="U11" s="2"/>
+      <c r="U11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
@@ -9213,7 +10313,7 @@
         <v>35</v>
       </c>
       <c r="P12" s="1"/>
-      <c r="U12" s="2"/>
+      <c r="U12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
@@ -9224,120 +10324,120 @@
         <v>40</v>
       </c>
       <c r="P13" s="1"/>
-      <c r="U13" s="2"/>
+      <c r="U13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="P14" s="1"/>
-      <c r="U14" s="2"/>
+      <c r="U14" s="3"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F15" s="1"/>
       <c r="P15" s="1"/>
-      <c r="U15" s="2"/>
+      <c r="U15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F16" s="1"/>
       <c r="P16" s="1"/>
-      <c r="U16" s="2"/>
+      <c r="U16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F17" s="1"/>
       <c r="P17" s="1"/>
-      <c r="U17" s="2"/>
+      <c r="U17" s="3"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F18" s="1"/>
       <c r="P18" s="1"/>
-      <c r="U18" s="2"/>
+      <c r="U18" s="3"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F19" s="1"/>
       <c r="L19" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="P19" s="1"/>
-      <c r="U19" s="2"/>
+      <c r="U19" s="3"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L20" s="0" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="U20" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="U20" s="3"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C21" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="E21" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E21" s="0" t="s">
-        <v>13</v>
-      </c>
       <c r="F21" s="1" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="G21" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="H21" s="0" t="s">
+      <c r="I21" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="I21" s="0" t="s">
+      <c r="K21" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="L21" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="M21" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="N21" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="O21" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="P21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K21" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="L21" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="M21" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="N21" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="O21" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="P21" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="Q21" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="R21" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="R21" s="0" t="s">
+      <c r="S21" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="S21" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="U21" s="2"/>
+      <c r="U21" s="3"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
@@ -9348,7 +10448,7 @@
         <v>0</v>
       </c>
       <c r="P22" s="1"/>
-      <c r="U22" s="2"/>
+      <c r="U22" s="3"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
@@ -9359,7 +10459,7 @@
         <v>5</v>
       </c>
       <c r="P23" s="1"/>
-      <c r="U23" s="2"/>
+      <c r="U23" s="3"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
@@ -9370,7 +10470,7 @@
         <v>10</v>
       </c>
       <c r="P24" s="1"/>
-      <c r="U24" s="2"/>
+      <c r="U24" s="3"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
@@ -9381,7 +10481,7 @@
         <v>15</v>
       </c>
       <c r="P25" s="1"/>
-      <c r="U25" s="2"/>
+      <c r="U25" s="3"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
@@ -9392,7 +10492,7 @@
         <v>20</v>
       </c>
       <c r="P26" s="1"/>
-      <c r="U26" s="2"/>
+      <c r="U26" s="3"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
@@ -9444,82 +10544,82 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F33" s="1"/>
       <c r="L33" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="P33" s="1"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L34" s="0" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C35" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D35" s="0" t="s">
+      <c r="E35" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E35" s="0" t="s">
-        <v>13</v>
-      </c>
       <c r="F35" s="1" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="G35" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H35" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="H35" s="0" t="s">
+      <c r="I35" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="I35" s="0" t="s">
+      <c r="K35" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="L35" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="M35" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="N35" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="O35" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="P35" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K35" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="L35" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="M35" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="N35" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="O35" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="P35" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="Q35" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="R35" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="R35" s="0" t="s">
+      <c r="S35" s="0" t="s">
         <v>16</v>
-      </c>
-      <c r="S35" s="0" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9604,92 +10704,92 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F44" s="1"/>
       <c r="K44" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P44" s="1"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F46" s="1"/>
       <c r="L46" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P46" s="1"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="0" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L47" s="0" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P47" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C48" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D48" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D48" s="0" t="s">
+      <c r="E48" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E48" s="0" t="s">
-        <v>13</v>
-      </c>
       <c r="F48" s="1" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="G48" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H48" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="H48" s="0" t="s">
+      <c r="I48" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="I48" s="0" t="s">
+      <c r="K48" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="L48" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="M48" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="N48" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="O48" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="P48" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K48" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="L48" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="M48" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="N48" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="O48" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="P48" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="Q48" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="R48" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="R48" s="0" t="s">
+      <c r="S48" s="0" t="s">
         <v>16</v>
-      </c>
-      <c r="S48" s="0" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9768,15 +10868,15 @@
       </c>
       <c r="F56" s="1"/>
       <c r="K56" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P56" s="1"/>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="F57" s="4"/>
+        <v>35</v>
+      </c>
+      <c r="F57" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>